<commit_message>
Update Capstone Gantt Chart
</commit_message>
<xml_diff>
--- a/Capstone Gantt Chart.xlsx
+++ b/Capstone Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\AndroidStudioProjects\A-Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E0258F-D89D-435E-A1B6-8400636BC3D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D529C024-A912-4442-825E-6C3D2FF6E244}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12398" windowHeight="5670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capston Schedule" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
   <si>
     <t>TASK NAME</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Chris</t>
-  </si>
-  <si>
-    <t>Rohan/Akash</t>
   </si>
   <si>
     <t>Akash</t>
@@ -736,6 +733,21 @@
     <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,21 +759,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,8 +1078,8 @@
   </sheetPr>
   <dimension ref="A1:BK996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1096,16 +1093,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15.75" customHeight="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1163,14 +1160,14 @@
       <c r="BK1" s="2"/>
     </row>
     <row r="2" spans="1:63" ht="15.75" customHeight="1">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1228,14 +1225,14 @@
       <c r="BK2" s="2"/>
     </row>
     <row r="3" spans="1:63" ht="30" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1293,115 +1290,115 @@
       <c r="BK3" s="7"/>
     </row>
     <row r="4" spans="1:63" ht="14.25">
-      <c r="A4" s="99"/>
-      <c r="B4" s="99" t="s">
+      <c r="A4" s="96"/>
+      <c r="B4" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="99" t="s">
+      <c r="E4" s="96" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="99" t="s">
+      <c r="G4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="104" t="s">
+      <c r="H4" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="103" t="s">
+      <c r="I4" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="101" t="s">
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="101" t="s">
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="95"/>
+      <c r="X4" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="101" t="s">
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="102"/>
-      <c r="AC4" s="101" t="s">
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="AD4" s="102"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="102"/>
-      <c r="AG4" s="102"/>
-      <c r="AH4" s="101" t="s">
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="AI4" s="102"/>
-      <c r="AJ4" s="102"/>
-      <c r="AK4" s="102"/>
-      <c r="AL4" s="102"/>
-      <c r="AM4" s="101" t="s">
+      <c r="AN4" s="95"/>
+      <c r="AO4" s="95"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="AN4" s="102"/>
-      <c r="AO4" s="102"/>
-      <c r="AP4" s="102"/>
-      <c r="AQ4" s="102"/>
-      <c r="AR4" s="101" t="s">
+      <c r="AS4" s="95"/>
+      <c r="AT4" s="95"/>
+      <c r="AU4" s="95"/>
+      <c r="AV4" s="95"/>
+      <c r="AW4" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="AS4" s="102"/>
-      <c r="AT4" s="102"/>
-      <c r="AU4" s="102"/>
-      <c r="AV4" s="102"/>
-      <c r="AW4" s="101" t="s">
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="95"/>
+      <c r="AZ4" s="95"/>
+      <c r="BA4" s="95"/>
+      <c r="BB4" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="AX4" s="102"/>
-      <c r="AY4" s="102"/>
-      <c r="AZ4" s="102"/>
-      <c r="BA4" s="102"/>
-      <c r="BB4" s="101" t="s">
+      <c r="BC4" s="95"/>
+      <c r="BD4" s="95"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="95"/>
+      <c r="BG4" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="BC4" s="102"/>
-      <c r="BD4" s="102"/>
-      <c r="BE4" s="102"/>
-      <c r="BF4" s="102"/>
-      <c r="BG4" s="101" t="s">
-        <v>49</v>
-      </c>
-      <c r="BH4" s="102"/>
-      <c r="BI4" s="102"/>
-      <c r="BJ4" s="102"/>
-      <c r="BK4" s="102"/>
+      <c r="BH4" s="95"/>
+      <c r="BI4" s="95"/>
+      <c r="BJ4" s="95"/>
+      <c r="BK4" s="95"/>
     </row>
     <row r="5" spans="1:63" ht="14.25">
-      <c r="A5" s="100"/>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="105"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="100"/>
       <c r="I5" s="37" t="s">
         <v>6</v>
       </c>
@@ -1573,12 +1570,12 @@
         <v>14</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
@@ -1637,7 +1634,7 @@
     </row>
     <row r="7" spans="1:63" ht="14.25">
       <c r="B7" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="29">
         <v>43494</v>
@@ -1814,7 +1811,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="18">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="I9" s="84"/>
       <c r="J9" s="85"/>
@@ -2111,7 +2108,7 @@
     </row>
     <row r="13" spans="1:63" ht="14.25">
       <c r="B13" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="16">
         <v>43529</v>
@@ -2193,12 +2190,12 @@
         <v>15</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
       <c r="I14" s="26"/>
       <c r="J14" s="27"/>
       <c r="K14" s="28"/>
@@ -2273,7 +2270,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="30">
         <v>1</v>
@@ -2431,7 +2428,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17" s="30">
         <v>0.2</v>
@@ -2510,7 +2507,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" s="30">
         <v>0.3</v>
@@ -2573,7 +2570,7 @@
     </row>
     <row r="19" spans="1:63" s="36" customFormat="1" ht="14.25">
       <c r="B19" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="29">
         <v>43519</v>
@@ -2589,7 +2586,7 @@
         <v>21</v>
       </c>
       <c r="G19" s="52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="30">
         <v>0.3</v>
@@ -2655,12 +2652,12 @@
         <v>16</v>
       </c>
       <c r="B20" s="25"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="104"/>
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
       <c r="K20" s="28"/>
@@ -2735,7 +2732,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="31">
         <v>0.95</v>
@@ -2798,7 +2795,7 @@
     </row>
     <row r="22" spans="1:63" ht="14.25">
       <c r="B22" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="29">
         <v>43500</v>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="23" spans="1:63" ht="14.25">
       <c r="B23" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="29">
         <v>43512</v>
@@ -2956,7 +2953,7 @@
     </row>
     <row r="24" spans="1:63" s="36" customFormat="1" ht="14.25">
       <c r="B24" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="29">
         <v>43512</v>
@@ -3035,7 +3032,7 @@
     </row>
     <row r="25" spans="1:63" ht="14.25">
       <c r="B25" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="29">
         <v>43519</v>
@@ -3117,12 +3114,12 @@
         <v>17</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
       <c r="K26" s="28"/>
@@ -3181,7 +3178,7 @@
     </row>
     <row r="27" spans="1:63" ht="14.25">
       <c r="B27" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="29">
         <v>43494</v>
@@ -3200,7 +3197,7 @@
         <v>27</v>
       </c>
       <c r="H27" s="31">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="I27" s="58"/>
       <c r="J27" s="59"/>
@@ -3260,7 +3257,7 @@
     </row>
     <row r="28" spans="1:63" ht="14.25">
       <c r="B28" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="29">
         <v>43497</v>
@@ -3275,24 +3272,24 @@
         <f t="shared" ref="F28:F33" si="4">NETWORKDAYS(C28,D28)</f>
         <v>8</v>
       </c>
-      <c r="G28" s="55" t="s">
-        <v>29</v>
+      <c r="G28" s="57" t="s">
+        <v>51</v>
       </c>
       <c r="H28" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="20"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="72"/>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="72"/>
+      <c r="R28" s="72"/>
+      <c r="S28" s="74"/>
+      <c r="T28" s="74"/>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
       <c r="W28" s="21"/>
@@ -3339,7 +3336,7 @@
     </row>
     <row r="29" spans="1:63" s="36" customFormat="1" ht="14.25">
       <c r="B29" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="29">
         <v>43509</v>
@@ -3418,7 +3415,7 @@
     </row>
     <row r="30" spans="1:63" s="36" customFormat="1" ht="14.25">
       <c r="B30" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="29">
         <v>43549</v>
@@ -3434,7 +3431,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H30" s="31">
         <v>0</v>
@@ -3497,7 +3494,7 @@
     </row>
     <row r="31" spans="1:63" ht="14.25">
       <c r="B31" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="29">
         <v>43529</v>
@@ -3576,7 +3573,7 @@
     </row>
     <row r="32" spans="1:63" s="46" customFormat="1" ht="14.25">
       <c r="B32" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="29">
         <v>43529</v>
@@ -3655,7 +3652,7 @@
     </row>
     <row r="33" spans="1:63" ht="14.25">
       <c r="B33" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="29">
         <v>43529</v>
@@ -3671,7 +3668,7 @@
         <v>27</v>
       </c>
       <c r="G33" s="57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H33" s="31">
         <v>0</v>
@@ -6692,6 +6689,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="AM4:AQ4"/>
     <mergeCell ref="AH4:AL4"/>
     <mergeCell ref="C4:C5"/>
@@ -6706,16 +6713,6 @@
     <mergeCell ref="BB4:BF4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:H19">
     <cfRule type="colorScale" priority="5">

</xml_diff>